<commit_message>
Skills 11134-11138. Contributed by ishand.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/stats/skills/SkillsToDo.xlsx
+++ b/trunk/dist/game/data/stats/skills/SkillsToDo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="637">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="G2" s="2">
         <f>COUNTIF(C2:C679,"yes")</f>
-        <v>553</v>
+        <v>558</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="G3">
         <f>678-G2</f>
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="G4" s="4">
         <f>100-(G3*100)/678</f>
-        <v>81.56342182890856</v>
+        <v>82.30088495575221</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6514,7 +6514,9 @@
       <c r="B349" s="7">
         <v>11134</v>
       </c>
-      <c r="C349" s="14"/>
+      <c r="C349" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D349" s="13"/>
     </row>
     <row r="350" spans="1:4">
@@ -6524,7 +6526,9 @@
       <c r="B350" s="7">
         <v>11135</v>
       </c>
-      <c r="C350" s="14"/>
+      <c r="C350" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D350" s="12"/>
     </row>
     <row r="351" spans="1:4">
@@ -6534,7 +6538,9 @@
       <c r="B351" s="7">
         <v>11136</v>
       </c>
-      <c r="C351" s="14"/>
+      <c r="C351" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D351" s="13"/>
     </row>
     <row r="352" spans="1:4">
@@ -6544,7 +6550,9 @@
       <c r="B352" s="7">
         <v>11137</v>
       </c>
-      <c r="C352" s="14"/>
+      <c r="C352" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D352" s="13"/>
     </row>
     <row r="353" spans="1:4">
@@ -6554,7 +6562,9 @@
       <c r="B353" s="7">
         <v>11138</v>
       </c>
-      <c r="C353" s="14"/>
+      <c r="C353" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D353" s="13"/>
     </row>
     <row r="354" spans="1:4">

</xml_diff>

<commit_message>
Call Skill Frost Trap, Gravity Trap and NPCs. Contributed by ishand.
</commit_message>
<xml_diff>
--- a/trunk/dist/game/data/stats/skills/SkillsToDo.xlsx
+++ b/trunk/dist/game/data/stats/skills/SkillsToDo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="637">
   <si>
     <t>Skill Name</t>
   </si>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="G2" s="2">
         <f>COUNTIF(C2:C679,"yes")</f>
-        <v>558</v>
+        <v>568</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="G3">
         <f>678-G2</f>
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="G4" s="4">
         <f>100-(G3*100)/678</f>
-        <v>82.30088495575221</v>
+        <v>83.775811209439524</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5632,7 +5632,9 @@
       <c r="B271" s="7">
         <v>10791</v>
       </c>
-      <c r="C271" s="14"/>
+      <c r="C271" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D271" s="13"/>
     </row>
     <row r="272" spans="1:4">
@@ -5642,7 +5644,9 @@
       <c r="B272" s="7">
         <v>10792</v>
       </c>
-      <c r="C272" s="14"/>
+      <c r="C272" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D272" s="12"/>
     </row>
     <row r="273" spans="1:4">
@@ -6606,7 +6610,9 @@
       <c r="B357" s="7">
         <v>11177</v>
       </c>
-      <c r="C357" s="14"/>
+      <c r="C357" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D357" s="12"/>
     </row>
     <row r="358" spans="1:4">
@@ -7530,7 +7536,9 @@
       <c r="B438" s="7">
         <v>11369</v>
       </c>
-      <c r="C438" s="14"/>
+      <c r="C438" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D438" s="13"/>
     </row>
     <row r="439" spans="1:4">
@@ -7540,7 +7548,9 @@
       <c r="B439" s="7">
         <v>11370</v>
       </c>
-      <c r="C439" s="14"/>
+      <c r="C439" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D439" s="12"/>
     </row>
     <row r="440" spans="1:4">
@@ -7550,7 +7560,9 @@
       <c r="B440" s="7">
         <v>11371</v>
       </c>
-      <c r="C440" s="14"/>
+      <c r="C440" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D440" s="12"/>
     </row>
     <row r="441" spans="1:4">
@@ -7560,7 +7572,9 @@
       <c r="B441" s="7">
         <v>11372</v>
       </c>
-      <c r="C441" s="14"/>
+      <c r="C441" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D441" s="13"/>
     </row>
     <row r="442" spans="1:4">
@@ -7570,7 +7584,9 @@
       <c r="B442" s="7">
         <v>11373</v>
       </c>
-      <c r="C442" s="14"/>
+      <c r="C442" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D442" s="13"/>
     </row>
     <row r="443" spans="1:4">
@@ -7580,7 +7596,9 @@
       <c r="B443" s="7">
         <v>11374</v>
       </c>
-      <c r="C443" s="14"/>
+      <c r="C443" s="14" t="s">
+        <v>548</v>
+      </c>
       <c r="D443" s="13"/>
     </row>
     <row r="444" spans="1:4">
@@ -9456,7 +9474,9 @@
       <c r="B603" s="7">
         <v>19203</v>
       </c>
-      <c r="C603" s="14"/>
+      <c r="C603" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="D603" s="12"/>
     </row>
     <row r="604" spans="1:4">

</xml_diff>